<commit_message>
Results from July 08, 2020 06:13:49 PM America/Chicago TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-08.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-08.xlsx
@@ -521,29 +521,15 @@
           <t>Texas</t>
         </is>
       </c>
-      <c r="B2" s="2" t="n">
-        <v>44019</v>
-      </c>
-      <c r="C2" t="n">
-        <v>23607</v>
-      </c>
-      <c r="D2" t="n">
-        <v>689</v>
-      </c>
-      <c r="E2" t="n">
-        <v>2747</v>
-      </c>
-      <c r="F2" t="n">
-        <v>89</v>
-      </c>
-      <c r="G2" t="n">
-        <v>0.12</v>
-      </c>
-      <c r="H2" t="n">
-        <v>0.13</v>
-      </c>
+      <c r="B2" t="inlineStr"/>
+      <c r="C2" t="inlineStr"/>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr"/>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
       <c r="I2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -558,7 +544,7 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... KeyError("None of ['Race/Ethnicity'] are in the columns")</t>
         </is>
       </c>
     </row>
@@ -620,29 +606,29 @@
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>214371</t>
+          <t>214570</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>18611</t>
+          <t>18618</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>33277</v>
+        <v>33320</v>
       </c>
       <c r="F4" t="n">
-        <v>5206</v>
+        <v>5210</v>
       </c>
       <c r="G4" t="n">
         <v>30.16</v>
       </c>
       <c r="H4" t="n">
-        <v>30.51</v>
+        <v>30.52</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
@@ -651,10 +637,10 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
-        <v>110332</v>
+        <v>110482</v>
       </c>
       <c r="L4" t="n">
-        <v>17065</v>
+        <v>17070</v>
       </c>
       <c r="M4" t="n">
         <v>2049418</v>
@@ -726,25 +712,25 @@
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C6" t="n">
-        <v>53514</v>
+        <v>55986</v>
       </c>
       <c r="D6" t="n">
-        <v>665</v>
+        <v>685</v>
       </c>
       <c r="E6" t="n">
-        <v>10872</v>
+        <v>11560</v>
       </c>
       <c r="F6" t="n">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="G6" t="n">
-        <v>20.32</v>
+        <v>20.65</v>
       </c>
       <c r="H6" t="n">
-        <v>35.19</v>
+        <v>35.18</v>
       </c>
       <c r="I6" t="b">
         <v>1</v>
@@ -773,21 +759,21 @@
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>26033</t>
+          <t>26755</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>194</t>
+          <t>201</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>666</t>
+          <t>689</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -826,25 +812,25 @@
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C8" t="n">
-        <v>17519</v>
+        <v>17919</v>
       </c>
       <c r="D8" t="n">
-        <v>602</v>
+        <v>608</v>
       </c>
       <c r="E8" t="n">
-        <v>1675</v>
+        <v>1707</v>
       </c>
       <c r="F8" t="n">
         <v>87</v>
       </c>
       <c r="G8" t="n">
-        <v>13.64</v>
+        <v>13.77</v>
       </c>
       <c r="H8" t="n">
-        <v>15.43</v>
+        <v>15.41</v>
       </c>
       <c r="I8" t="b">
         <v>0</v>
@@ -853,10 +839,10 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
-        <v>12280</v>
+        <v>12399</v>
       </c>
       <c r="L8" t="n">
-        <v>564</v>
+        <v>570</v>
       </c>
       <c r="M8" t="n">
         <v>354112</v>
@@ -877,7 +863,7 @@
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C9" t="n">
         <v>24512</v>
@@ -1026,16 +1012,16 @@
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C12" t="n">
-        <v>13727</v>
+        <v>14017</v>
       </c>
       <c r="D12" t="n">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="E12" t="n">
-        <v>261</v>
+        <v>266</v>
       </c>
       <c r="F12" t="inlineStr"/>
       <c r="G12" t="n">
@@ -1210,25 +1196,25 @@
         </is>
       </c>
       <c r="B16" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C16" t="n">
-        <v>120539</v>
+        <v>123004</v>
       </c>
       <c r="D16" t="n">
-        <v>3579</v>
+        <v>3642</v>
       </c>
       <c r="E16" t="n">
-        <v>3232</v>
+        <v>3310</v>
       </c>
       <c r="F16" t="n">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="G16" t="n">
-        <v>4.7</v>
+        <v>4.74</v>
       </c>
       <c r="H16" t="n">
-        <v>11.09</v>
+        <v>10.98</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1237,10 +1223,10 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>68774</v>
+        <v>69866</v>
       </c>
       <c r="L16" t="n">
-        <v>3327</v>
+        <v>3389</v>
       </c>
       <c r="M16" t="n">
         <v>823987</v>
@@ -1312,25 +1298,25 @@
         </is>
       </c>
       <c r="B18" s="2" t="n">
-        <v>44018</v>
+        <v>44019</v>
       </c>
       <c r="C18" t="n">
-        <v>32214</v>
+        <v>32888</v>
       </c>
       <c r="D18" t="n">
-        <v>1158</v>
+        <v>1188</v>
       </c>
       <c r="E18" t="n">
-        <v>15391</v>
+        <v>15720</v>
       </c>
       <c r="F18" t="n">
-        <v>579</v>
+        <v>595</v>
       </c>
       <c r="G18" t="n">
-        <v>47.78</v>
+        <v>47.8</v>
       </c>
       <c r="H18" t="n">
-        <v>50</v>
+        <v>50.08</v>
       </c>
       <c r="I18" t="b">
         <v>1</v>
@@ -1551,25 +1537,25 @@
         </is>
       </c>
       <c r="B23" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C23" t="n">
-        <v>34664</v>
+        <v>35116</v>
       </c>
       <c r="D23" t="n">
-        <v>1696</v>
+        <v>1704</v>
       </c>
       <c r="E23" t="n">
-        <v>1827</v>
+        <v>1840</v>
       </c>
       <c r="F23" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="G23" t="n">
-        <v>6.42</v>
+        <v>6.39</v>
       </c>
       <c r="H23" t="n">
-        <v>6.73</v>
+        <v>6.75</v>
       </c>
       <c r="I23" t="b">
         <v>0</v>
@@ -1578,10 +1564,10 @@
         <v>0</v>
       </c>
       <c r="K23" t="n">
-        <v>28456</v>
+        <v>28809</v>
       </c>
       <c r="L23" t="n">
-        <v>1634</v>
+        <v>1644</v>
       </c>
       <c r="M23" t="n">
         <v>227938</v>
@@ -1602,22 +1588,22 @@
         </is>
       </c>
       <c r="B24" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C24" t="n">
-        <v>20201</v>
+        <v>20425</v>
       </c>
       <c r="D24" t="n">
         <v>282</v>
       </c>
       <c r="E24" t="n">
-        <v>1200</v>
+        <v>1205</v>
       </c>
       <c r="F24" t="n">
         <v>21</v>
       </c>
       <c r="G24" t="n">
-        <v>7.67</v>
+        <v>7.63</v>
       </c>
       <c r="H24" t="n">
         <v>7.72</v>
@@ -1629,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>15643</v>
+        <v>15786</v>
       </c>
       <c r="L24" t="n">
         <v>272</v>
@@ -1653,22 +1639,22 @@
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C25" t="n">
-        <v>66540</v>
+        <v>67153</v>
       </c>
       <c r="D25" t="n">
-        <v>5926</v>
+        <v>5934</v>
       </c>
       <c r="E25" t="n">
-        <v>20100</v>
+        <v>20210</v>
       </c>
       <c r="F25" t="n">
-        <v>2364</v>
+        <v>2367</v>
       </c>
       <c r="G25" t="n">
-        <v>30.21</v>
+        <v>30.1</v>
       </c>
       <c r="H25" t="n">
         <v>39.89</v>
@@ -1798,22 +1784,22 @@
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C28" t="n">
-        <v>1184</v>
+        <v>1226</v>
       </c>
       <c r="D28" t="n">
         <v>17</v>
       </c>
       <c r="E28" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
       </c>
       <c r="G28" t="n">
-        <v>1.4</v>
+        <v>1.41</v>
       </c>
       <c r="H28" t="n">
         <v>0</v>
@@ -1825,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>2069</v>
+        <v>2135</v>
       </c>
       <c r="L28" t="n">
         <v>34</v>
@@ -1849,25 +1835,25 @@
         </is>
       </c>
       <c r="B29" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C29" t="n">
-        <v>32556</v>
+        <v>33154</v>
       </c>
       <c r="D29" t="n">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="E29" t="n">
-        <v>5560</v>
+        <v>5634</v>
       </c>
       <c r="F29" t="n">
         <v>192</v>
       </c>
       <c r="G29" t="n">
-        <v>18.97</v>
+        <v>18.88</v>
       </c>
       <c r="H29" t="n">
-        <v>24.21</v>
+        <v>24.15</v>
       </c>
       <c r="I29" t="b">
         <v>0</v>
@@ -1876,10 +1862,10 @@
         <v>1</v>
       </c>
       <c r="K29" t="n">
-        <v>29315</v>
+        <v>29848</v>
       </c>
       <c r="L29" t="n">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="M29" t="n">
         <v>368744</v>
@@ -1900,22 +1886,22 @@
         </is>
       </c>
       <c r="B30" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C30" t="n">
-        <v>100470</v>
+        <v>103890</v>
       </c>
       <c r="D30" t="n">
-        <v>2899</v>
+        <v>2922</v>
       </c>
       <c r="E30" t="n">
-        <v>27660</v>
+        <v>28382</v>
       </c>
       <c r="F30" t="n">
-        <v>1361</v>
+        <v>1372</v>
       </c>
       <c r="G30" t="n">
-        <v>27.53</v>
+        <v>27.32</v>
       </c>
       <c r="H30" t="n">
         <v>46.95</v>
@@ -1947,16 +1933,16 @@
         </is>
       </c>
       <c r="B31" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C31" t="n">
-        <v>37420</v>
+        <v>37941</v>
       </c>
       <c r="D31" t="n">
-        <v>1384</v>
+        <v>1394</v>
       </c>
       <c r="E31" t="n">
-        <v>1464</v>
+        <v>1478</v>
       </c>
       <c r="F31" t="n">
         <v>45</v>
@@ -1965,7 +1951,7 @@
         <v>5.48</v>
       </c>
       <c r="H31" t="n">
-        <v>3.43</v>
+        <v>3.4</v>
       </c>
       <c r="I31" t="b">
         <v>0</v>
@@ -1974,10 +1960,10 @@
         <v>0</v>
       </c>
       <c r="K31" t="n">
-        <v>26717</v>
+        <v>26965</v>
       </c>
       <c r="L31" t="n">
-        <v>1312</v>
+        <v>1323</v>
       </c>
       <c r="M31" t="n">
         <v>269854</v>
@@ -2045,25 +2031,25 @@
         </is>
       </c>
       <c r="B33" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C33" t="n">
-        <v>12414</v>
+        <v>12462</v>
       </c>
       <c r="D33" t="n">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="E33" t="n">
-        <v>3174</v>
+        <v>3197</v>
       </c>
       <c r="F33" t="n">
         <v>131</v>
       </c>
       <c r="G33" t="n">
-        <v>25.57</v>
+        <v>25.65</v>
       </c>
       <c r="H33" t="n">
-        <v>25.49</v>
+        <v>25.44</v>
       </c>
       <c r="I33" t="b">
         <v>1</v>
@@ -2221,25 +2207,25 @@
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C37" t="n">
-        <v>148452</v>
+        <v>149432</v>
       </c>
       <c r="D37" t="n">
-        <v>7063</v>
+        <v>7099</v>
       </c>
       <c r="E37" t="n">
-        <v>24901</v>
+        <v>25072</v>
       </c>
       <c r="F37" t="n">
-        <v>1965</v>
+        <v>1967</v>
       </c>
       <c r="G37" t="n">
-        <v>16.77</v>
+        <v>16.78</v>
       </c>
       <c r="H37" t="n">
-        <v>27.82</v>
+        <v>27.71</v>
       </c>
       <c r="I37" t="b">
         <v>1</v>
@@ -2268,16 +2254,16 @@
         </is>
       </c>
       <c r="B38" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C38" t="n">
-        <v>8539</v>
+        <v>8969</v>
       </c>
       <c r="D38" t="n">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="E38" t="n">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F38" t="n">
         <v>1</v>
@@ -2286,7 +2272,7 @@
         <v>1.49</v>
       </c>
       <c r="H38" t="n">
-        <v>1.06</v>
+        <v>1.02</v>
       </c>
       <c r="I38" t="b">
         <v>0</v>
@@ -2362,25 +2348,25 @@
         </is>
       </c>
       <c r="B40" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C40" t="n">
-        <v>110338</v>
+        <v>110602</v>
       </c>
       <c r="D40" t="n">
-        <v>8213</v>
+        <v>8243</v>
       </c>
       <c r="E40" t="n">
-        <v>10400</v>
+        <v>10414</v>
       </c>
       <c r="F40" t="n">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="G40" t="n">
-        <v>9.43</v>
+        <v>9.42</v>
       </c>
       <c r="H40" t="n">
-        <v>8.18</v>
+        <v>8.19</v>
       </c>
       <c r="I40" t="b">
         <v>1</v>
@@ -2409,22 +2395,22 @@
         </is>
       </c>
       <c r="B41" s="2" t="n">
-        <v>44019</v>
+        <v>44020</v>
       </c>
       <c r="C41" t="n">
-        <v>12577</v>
+        <v>12834</v>
       </c>
       <c r="D41" t="n">
         <v>358</v>
       </c>
       <c r="E41" t="n">
-        <v>3635</v>
+        <v>3731</v>
       </c>
       <c r="F41" t="n">
         <v>145</v>
       </c>
       <c r="G41" t="n">
-        <v>31.14</v>
+        <v>31.32</v>
       </c>
       <c r="H41" t="n">
         <v>40.5</v>
@@ -2436,7 +2422,7 @@
         <v>0</v>
       </c>
       <c r="K41" t="n">
-        <v>11673</v>
+        <v>11914</v>
       </c>
       <c r="L41" t="n">
         <v>358</v>

</xml_diff>

<commit_message>
Results from July 08, 2020 11:01:00 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-08.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-08.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -56,11 +59,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -426,7 +430,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -514,7 +518,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B2" t="inlineStr"/>
@@ -533,47 +537,1956 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>109911</v>
+        <v>3365783</v>
       </c>
       <c r="N2" t="n">
-        <v>3.51</v>
+        <v>12.07</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>An error occurred. ... ValueError('Unable to parse "Reported Deaths In Adair : No Data" as int')</t>
+          <t>An error occurred. ... KeyError("None of ['Race/Ethnicity'] are in the columns")</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Texas</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr"/>
-      <c r="D3" t="inlineStr"/>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr"/>
-      <c r="G3" t="inlineStr"/>
-      <c r="H3" t="inlineStr"/>
+          <t>Texas -- Bexar County</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C3" t="n">
+        <v>16725</v>
+      </c>
+      <c r="D3" t="n">
+        <v>146</v>
+      </c>
+      <c r="E3" t="n">
+        <v>464</v>
+      </c>
+      <c r="F3" t="n">
+        <v>17</v>
+      </c>
+      <c r="G3" t="n">
+        <v>6.81</v>
+      </c>
+      <c r="H3" t="n">
+        <v>15.32</v>
+      </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="J3" t="b">
         <v>0</v>
       </c>
-      <c r="K3" t="inlineStr"/>
-      <c r="L3" t="inlineStr"/>
+      <c r="K3" t="n">
+        <v>6812</v>
+      </c>
+      <c r="L3" t="n">
+        <v>111</v>
+      </c>
       <c r="M3" t="n">
-        <v>3365783</v>
+        <v>146703</v>
       </c>
       <c r="N3" t="n">
-        <v>12.07</v>
+        <v>7.62</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>An error occurred. ... KeyError("None of ['Race/Ethnicity'] are in the columns")</t>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>New York -- New York</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>214570</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>18618</t>
+        </is>
+      </c>
+      <c r="E4" t="n">
+        <v>33320</v>
+      </c>
+      <c r="F4" t="n">
+        <v>5210</v>
+      </c>
+      <c r="G4" t="n">
+        <v>30.16</v>
+      </c>
+      <c r="H4" t="n">
+        <v>30.52</v>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="n">
+        <v>110482</v>
+      </c>
+      <c r="L4" t="n">
+        <v>17070</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2049418</v>
+      </c>
+      <c r="N4" t="n">
+        <v>24.27</v>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Rhode Island</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>44015</v>
+      </c>
+      <c r="C5" t="n">
+        <v>16491</v>
+      </c>
+      <c r="D5" t="n">
+        <v>960</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1592</v>
+      </c>
+      <c r="F5" t="n">
+        <v>48</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12.29</v>
+      </c>
+      <c r="H5" t="n">
+        <v>6.14</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="b">
+        <v>0</v>
+      </c>
+      <c r="K5" t="n">
+        <v>12950</v>
+      </c>
+      <c r="L5" t="n">
+        <v>782</v>
+      </c>
+      <c r="M5" t="n">
+        <v>69254</v>
+      </c>
+      <c r="N5" t="n">
+        <v>6.55</v>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Tennessee</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C6" t="n">
+        <v>55986</v>
+      </c>
+      <c r="D6" t="n">
+        <v>685</v>
+      </c>
+      <c r="E6" t="n">
+        <v>11560</v>
+      </c>
+      <c r="F6" t="n">
+        <v>241</v>
+      </c>
+      <c r="G6" t="n">
+        <v>20.65</v>
+      </c>
+      <c r="H6" t="n">
+        <v>35.18</v>
+      </c>
+      <c r="I6" t="b">
+        <v>1</v>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="n">
+        <v>1117489</v>
+      </c>
+      <c r="N6" t="n">
+        <v>16.8</v>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>26755</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>201</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>689</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>&lt;5</t>
+        </is>
+      </c>
+      <c r="G7" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="b">
+        <v>1</v>
+      </c>
+      <c r="J7" t="b">
+        <v>0</v>
+      </c>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="n">
+        <v>35862</v>
+      </c>
+      <c r="N7" t="n">
+        <v>1.18</v>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Kentucky</t>
+        </is>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C8" t="n">
+        <v>17919</v>
+      </c>
+      <c r="D8" t="n">
+        <v>608</v>
+      </c>
+      <c r="E8" t="n">
+        <v>1707</v>
+      </c>
+      <c r="F8" t="n">
+        <v>87</v>
+      </c>
+      <c r="G8" t="n">
+        <v>13.77</v>
+      </c>
+      <c r="H8" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>12399</v>
+      </c>
+      <c r="L8" t="n">
+        <v>570</v>
+      </c>
+      <c r="M8" t="n">
+        <v>354112</v>
+      </c>
+      <c r="N8" t="n">
+        <v>7.98</v>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Arkansas</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C9" t="n">
+        <v>25246</v>
+      </c>
+      <c r="D9" t="n">
+        <v>305</v>
+      </c>
+      <c r="E9" t="n">
+        <v>5471</v>
+      </c>
+      <c r="F9" t="n">
+        <v>74</v>
+      </c>
+      <c r="G9" t="n">
+        <v>25.07</v>
+      </c>
+      <c r="H9" t="n">
+        <v>25.69</v>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>21820</v>
+      </c>
+      <c r="L9" t="n">
+        <v>288</v>
+      </c>
+      <c r="M9" t="n">
+        <v>460970</v>
+      </c>
+      <c r="N9" t="n">
+        <v>15.41</v>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>California - San Diego</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C10" t="n">
+        <v>17842</v>
+      </c>
+      <c r="D10" t="n">
+        <v>406</v>
+      </c>
+      <c r="E10" t="n">
+        <v>642</v>
+      </c>
+      <c r="F10" t="n">
+        <v>15</v>
+      </c>
+      <c r="G10" t="n">
+        <v>4.52</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="b">
+        <v>0</v>
+      </c>
+      <c r="K10" t="n">
+        <v>14190</v>
+      </c>
+      <c r="L10" t="n">
+        <v>399</v>
+      </c>
+      <c r="M10" t="n">
+        <v>166412</v>
+      </c>
+      <c r="N10" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C11" t="n">
+        <v>67375</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1905</v>
+      </c>
+      <c r="E11" t="n">
+        <v>9967</v>
+      </c>
+      <c r="F11" t="n">
+        <v>429</v>
+      </c>
+      <c r="G11" t="n">
+        <v>14.79</v>
+      </c>
+      <c r="H11" t="n">
+        <v>22.52</v>
+      </c>
+      <c r="I11" t="b">
+        <v>1</v>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
+      </c>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="n">
+        <v>1613285</v>
+      </c>
+      <c r="N11" t="n">
+        <v>19.17</v>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>New Mexico</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C12" t="n">
+        <v>14017</v>
+      </c>
+      <c r="D12" t="n">
+        <v>527</v>
+      </c>
+      <c r="E12" t="n">
+        <v>266</v>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="b">
+        <v>1</v>
+      </c>
+      <c r="J12" t="b">
+        <v>0</v>
+      </c>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="n">
+        <v>43006</v>
+      </c>
+      <c r="N12" t="n">
+        <v>2.06</v>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Florida -- Miami-Dade County</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C13" t="n">
+        <v>53974</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1068</v>
+      </c>
+      <c r="E13" t="n">
+        <v>6262</v>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="n">
+        <v>20.53</v>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>30505</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="n">
+        <v>481976</v>
+      </c>
+      <c r="N13" t="n">
+        <v>17.75</v>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Florida -- Orange County</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C14" t="n">
+        <v>15194</v>
+      </c>
+      <c r="D14" t="n">
+        <v>63</v>
+      </c>
+      <c r="E14" t="n">
+        <v>1975</v>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="n">
+        <v>24.35</v>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="n">
+        <v>8111</v>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>277193</v>
+      </c>
+      <c r="N14" t="n">
+        <v>20.98</v>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Alabama</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C15" t="n">
+        <v>46424</v>
+      </c>
+      <c r="D15" t="n">
+        <v>1032</v>
+      </c>
+      <c r="E15" t="n">
+        <v>16007</v>
+      </c>
+      <c r="F15" t="n">
+        <v>459</v>
+      </c>
+      <c r="G15" t="n">
+        <v>46.01</v>
+      </c>
+      <c r="H15" t="n">
+        <v>46.18</v>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="b">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>34792</v>
+      </c>
+      <c r="L15" t="n">
+        <v>994</v>
+      </c>
+      <c r="M15" t="n">
+        <v>1293186</v>
+      </c>
+      <c r="N15" t="n">
+        <v>26.58</v>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>California - Los Angeles</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>44019</v>
+      </c>
+      <c r="C16" t="n">
+        <v>123004</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3642</v>
+      </c>
+      <c r="E16" t="n">
+        <v>3310</v>
+      </c>
+      <c r="F16" t="n">
+        <v>372</v>
+      </c>
+      <c r="G16" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="H16" t="n">
+        <v>10.98</v>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="b">
+        <v>0</v>
+      </c>
+      <c r="K16" t="n">
+        <v>69866</v>
+      </c>
+      <c r="L16" t="n">
+        <v>3389</v>
+      </c>
+      <c r="M16" t="n">
+        <v>823987</v>
+      </c>
+      <c r="N16" t="n">
+        <v>8.16</v>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>Maryland</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C17" t="n">
+        <v>70861</v>
+      </c>
+      <c r="D17" t="n">
+        <v>3149</v>
+      </c>
+      <c r="E17" t="n">
+        <v>20288</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1270</v>
+      </c>
+      <c r="G17" t="n">
+        <v>28.63</v>
+      </c>
+      <c r="H17" t="n">
+        <v>40.33</v>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="b">
+        <v>0</v>
+      </c>
+      <c r="K17" t="n">
+        <v>57896</v>
+      </c>
+      <c r="L17" t="n">
+        <v>70838</v>
+      </c>
+      <c r="M17" t="n">
+        <v>1788090</v>
+      </c>
+      <c r="N17" t="n">
+        <v>29.78</v>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Mississippi</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>44019</v>
+      </c>
+      <c r="C18" t="n">
+        <v>32888</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1188</v>
+      </c>
+      <c r="E18" t="n">
+        <v>15720</v>
+      </c>
+      <c r="F18" t="n">
+        <v>595</v>
+      </c>
+      <c r="G18" t="n">
+        <v>47.8</v>
+      </c>
+      <c r="H18" t="n">
+        <v>50.08</v>
+      </c>
+      <c r="I18" t="b">
+        <v>1</v>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="n">
+        <v>1125834</v>
+      </c>
+      <c r="N18" t="n">
+        <v>37.67</v>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Pennsylvania</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C19" t="n">
+        <v>89515</v>
+      </c>
+      <c r="D19" t="n">
+        <v>6812</v>
+      </c>
+      <c r="E19" t="n">
+        <v>11886</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1426</v>
+      </c>
+      <c r="G19" t="n">
+        <v>30.04</v>
+      </c>
+      <c r="H19" t="n">
+        <v>21.68</v>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" t="n">
+        <v>39564</v>
+      </c>
+      <c r="L19" t="n">
+        <v>6579</v>
+      </c>
+      <c r="M19" t="n">
+        <v>1423319</v>
+      </c>
+      <c r="N19" t="n">
+        <v>11.13</v>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C20" t="n">
+        <v>220492</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3889</v>
+      </c>
+      <c r="E20" t="n">
+        <v>28460</v>
+      </c>
+      <c r="F20" t="n">
+        <v>764</v>
+      </c>
+      <c r="G20" t="n">
+        <v>12.91</v>
+      </c>
+      <c r="H20" t="n">
+        <v>19.65</v>
+      </c>
+      <c r="I20" t="b">
+        <v>1</v>
+      </c>
+      <c r="J20" t="b">
+        <v>0</v>
+      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="n">
+        <v>3316376</v>
+      </c>
+      <c r="N20" t="n">
+        <v>16.1</v>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Montana</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C21" t="n">
+        <v>1371</v>
+      </c>
+      <c r="D21" t="n">
+        <v>23</v>
+      </c>
+      <c r="E21" t="n">
+        <v>6</v>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="b">
+        <v>1</v>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="n">
+        <v>4630</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Vermont</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C22" t="n">
+        <v>1256</v>
+      </c>
+      <c r="D22" t="n">
+        <v>56</v>
+      </c>
+      <c r="E22" t="n">
+        <v>128</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>10.47</v>
+      </c>
+      <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" t="n">
+        <v>1223</v>
+      </c>
+      <c r="L22" t="n">
+        <v>56</v>
+      </c>
+      <c r="M22" t="n">
+        <v>8058</v>
+      </c>
+      <c r="N22" t="n">
+        <v>1.29</v>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Colorado</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C23" t="n">
+        <v>35116</v>
+      </c>
+      <c r="D23" t="n">
+        <v>1704</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1840</v>
+      </c>
+      <c r="F23" t="n">
+        <v>111</v>
+      </c>
+      <c r="G23" t="n">
+        <v>6.39</v>
+      </c>
+      <c r="H23" t="n">
+        <v>6.75</v>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="b">
+        <v>0</v>
+      </c>
+      <c r="K23" t="n">
+        <v>28809</v>
+      </c>
+      <c r="L23" t="n">
+        <v>1644</v>
+      </c>
+      <c r="M23" t="n">
+        <v>227938</v>
+      </c>
+      <c r="N23" t="n">
+        <v>4.12</v>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Nebraska</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C24" t="n">
+        <v>20425</v>
+      </c>
+      <c r="D24" t="n">
+        <v>282</v>
+      </c>
+      <c r="E24" t="n">
+        <v>1205</v>
+      </c>
+      <c r="F24" t="n">
+        <v>21</v>
+      </c>
+      <c r="G24" t="n">
+        <v>7.63</v>
+      </c>
+      <c r="H24" t="n">
+        <v>7.72</v>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="n">
+        <v>15786</v>
+      </c>
+      <c r="L24" t="n">
+        <v>272</v>
+      </c>
+      <c r="M24" t="n">
+        <v>90860</v>
+      </c>
+      <c r="N24" t="n">
+        <v>4.77</v>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Michigan</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C25" t="n">
+        <v>67153</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5934</v>
+      </c>
+      <c r="E25" t="n">
+        <v>20210</v>
+      </c>
+      <c r="F25" t="n">
+        <v>2367</v>
+      </c>
+      <c r="G25" t="n">
+        <v>30.1</v>
+      </c>
+      <c r="H25" t="n">
+        <v>39.89</v>
+      </c>
+      <c r="I25" t="b">
+        <v>1</v>
+      </c>
+      <c r="J25" t="b">
+        <v>0</v>
+      </c>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="n">
+        <v>1375424</v>
+      </c>
+      <c r="N25" t="n">
+        <v>13.81</v>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="n">
+        <v>44019</v>
+      </c>
+      <c r="C26" t="n">
+        <v>289468</v>
+      </c>
+      <c r="D26" t="n">
+        <v>6474</v>
+      </c>
+      <c r="E26" t="n">
+        <v>8125</v>
+      </c>
+      <c r="F26" t="n">
+        <v>582</v>
+      </c>
+      <c r="G26" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="H26" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="I26" t="b">
+        <v>0</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+      <c r="K26" t="n">
+        <v>185891</v>
+      </c>
+      <c r="L26" t="n">
+        <v>6375</v>
+      </c>
+      <c r="M26" t="n">
+        <v>2267875</v>
+      </c>
+      <c r="N26" t="n">
+        <v>5.79</v>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Indiana</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C27" t="n">
+        <v>49063</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2539</v>
+      </c>
+      <c r="E27" t="n">
+        <v>5905</v>
+      </c>
+      <c r="F27" t="n">
+        <v>368</v>
+      </c>
+      <c r="G27" t="n">
+        <v>12.04</v>
+      </c>
+      <c r="H27" t="n">
+        <v>14.49</v>
+      </c>
+      <c r="I27" t="b">
+        <v>1</v>
+      </c>
+      <c r="J27" t="b">
+        <v>1</v>
+      </c>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="n">
+        <v>619472</v>
+      </c>
+      <c r="N27" t="n">
+        <v>9.33</v>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Alaska</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1226</v>
+      </c>
+      <c r="D28" t="n">
+        <v>17</v>
+      </c>
+      <c r="E28" t="n">
+        <v>30</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>1.41</v>
+      </c>
+      <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="b">
+        <v>0</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+      <c r="K28" t="n">
+        <v>2135</v>
+      </c>
+      <c r="L28" t="n">
+        <v>34</v>
+      </c>
+      <c r="M28" t="n">
+        <v>24129</v>
+      </c>
+      <c r="N28" t="n">
+        <v>3.27</v>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C29" t="n">
+        <v>33154</v>
+      </c>
+      <c r="D29" t="n">
+        <v>807</v>
+      </c>
+      <c r="E29" t="n">
+        <v>5634</v>
+      </c>
+      <c r="F29" t="n">
+        <v>192</v>
+      </c>
+      <c r="G29" t="n">
+        <v>18.88</v>
+      </c>
+      <c r="H29" t="n">
+        <v>24.15</v>
+      </c>
+      <c r="I29" t="b">
+        <v>0</v>
+      </c>
+      <c r="J29" t="b">
+        <v>1</v>
+      </c>
+      <c r="K29" t="n">
+        <v>29848</v>
+      </c>
+      <c r="L29" t="n">
+        <v>795</v>
+      </c>
+      <c r="M29" t="n">
+        <v>368744</v>
+      </c>
+      <c r="N29" t="n">
+        <v>6.38</v>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C30" t="n">
+        <v>103890</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2922</v>
+      </c>
+      <c r="E30" t="n">
+        <v>28382</v>
+      </c>
+      <c r="F30" t="n">
+        <v>1372</v>
+      </c>
+      <c r="G30" t="n">
+        <v>27.32</v>
+      </c>
+      <c r="H30" t="n">
+        <v>46.95</v>
+      </c>
+      <c r="I30" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="n">
+        <v>3239300</v>
+      </c>
+      <c r="N30" t="n">
+        <v>31.46</v>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Washington</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C31" t="n">
+        <v>37941</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1394</v>
+      </c>
+      <c r="E31" t="n">
+        <v>1478</v>
+      </c>
+      <c r="F31" t="n">
+        <v>45</v>
+      </c>
+      <c r="G31" t="n">
+        <v>5.48</v>
+      </c>
+      <c r="H31" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="I31" t="b">
+        <v>0</v>
+      </c>
+      <c r="J31" t="b">
+        <v>0</v>
+      </c>
+      <c r="K31" t="n">
+        <v>26965</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1323</v>
+      </c>
+      <c r="M31" t="n">
+        <v>269854</v>
+      </c>
+      <c r="N31" t="n">
+        <v>3.7</v>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Washington, DC</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="n">
+        <v>44019</v>
+      </c>
+      <c r="C32" t="n">
+        <v>10569</v>
+      </c>
+      <c r="D32" t="n">
+        <v>561</v>
+      </c>
+      <c r="E32" t="n">
+        <v>5241</v>
+      </c>
+      <c r="F32" t="n">
+        <v>418</v>
+      </c>
+      <c r="G32" t="n">
+        <v>49.59</v>
+      </c>
+      <c r="H32" t="n">
+        <v>74.51000000000001</v>
+      </c>
+      <c r="I32" t="b">
+        <v>1</v>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="n">
+        <v>321317</v>
+      </c>
+      <c r="N32" t="n">
+        <v>46.94</v>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Delaware</t>
+        </is>
+      </c>
+      <c r="B33" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C33" t="n">
+        <v>12462</v>
+      </c>
+      <c r="D33" t="n">
+        <v>515</v>
+      </c>
+      <c r="E33" t="n">
+        <v>3197</v>
+      </c>
+      <c r="F33" t="n">
+        <v>131</v>
+      </c>
+      <c r="G33" t="n">
+        <v>25.65</v>
+      </c>
+      <c r="H33" t="n">
+        <v>25.44</v>
+      </c>
+      <c r="I33" t="b">
+        <v>1</v>
+      </c>
+      <c r="J33" t="b">
+        <v>0</v>
+      </c>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="n">
+        <v>209892</v>
+      </c>
+      <c r="N33" t="n">
+        <v>22.11</v>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Maine</t>
+        </is>
+      </c>
+      <c r="B34" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C34" t="n">
+        <v>3460</v>
+      </c>
+      <c r="D34" t="n">
+        <v>110</v>
+      </c>
+      <c r="E34" t="n">
+        <v>806</v>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="n">
+        <v>26.33</v>
+      </c>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="b">
+        <v>0</v>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
+      </c>
+      <c r="K34" t="n">
+        <v>3061</v>
+      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="n">
+        <v>17881</v>
+      </c>
+      <c r="N34" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Iowa</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr"/>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
+      <c r="E35" t="inlineStr"/>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" t="b">
+        <v>0</v>
+      </c>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="n">
+        <v>109911</v>
+      </c>
+      <c r="N35" t="n">
+        <v>3.51</v>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>An error occurred. ... ValueError('Unable to parse "Reported Deaths In Adair : No Data" as int')</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>North Carolina</t>
+        </is>
+      </c>
+      <c r="B36" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C36" t="n">
+        <v>77310</v>
+      </c>
+      <c r="D36" t="n">
+        <v>1441</v>
+      </c>
+      <c r="E36" t="n">
+        <v>12526</v>
+      </c>
+      <c r="F36" t="n">
+        <v>457</v>
+      </c>
+      <c r="G36" t="n">
+        <v>23.74</v>
+      </c>
+      <c r="H36" t="n">
+        <v>32.88</v>
+      </c>
+      <c r="I36" t="b">
+        <v>0</v>
+      </c>
+      <c r="J36" t="b">
+        <v>1</v>
+      </c>
+      <c r="K36" t="n">
+        <v>52756</v>
+      </c>
+      <c r="L36" t="n">
+        <v>1390</v>
+      </c>
+      <c r="M36" t="n">
+        <v>2179622</v>
+      </c>
+      <c r="N36" t="n">
+        <v>21.46</v>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Illinois</t>
+        </is>
+      </c>
+      <c r="B37" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C37" t="n">
+        <v>149432</v>
+      </c>
+      <c r="D37" t="n">
+        <v>7099</v>
+      </c>
+      <c r="E37" t="n">
+        <v>25072</v>
+      </c>
+      <c r="F37" t="n">
+        <v>1967</v>
+      </c>
+      <c r="G37" t="n">
+        <v>16.78</v>
+      </c>
+      <c r="H37" t="n">
+        <v>27.71</v>
+      </c>
+      <c r="I37" t="b">
+        <v>1</v>
+      </c>
+      <c r="J37" t="b">
+        <v>0</v>
+      </c>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="n">
+        <v>1824125</v>
+      </c>
+      <c r="N37" t="n">
+        <v>14.23</v>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Idaho</t>
+        </is>
+      </c>
+      <c r="B38" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C38" t="n">
+        <v>8969</v>
+      </c>
+      <c r="D38" t="n">
+        <v>98</v>
+      </c>
+      <c r="E38" t="n">
+        <v>134</v>
+      </c>
+      <c r="F38" t="n">
+        <v>1</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1.49</v>
+      </c>
+      <c r="H38" t="n">
+        <v>1.02</v>
+      </c>
+      <c r="I38" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
+      </c>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="n">
+        <v>11536</v>
+      </c>
+      <c r="N38" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Minnesota</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C39" t="n">
+        <v>39589</v>
+      </c>
+      <c r="D39" t="n">
+        <v>1485</v>
+      </c>
+      <c r="E39" t="n">
+        <v>8083</v>
+      </c>
+      <c r="F39" t="n">
+        <v>131</v>
+      </c>
+      <c r="G39" t="n">
+        <v>20.42</v>
+      </c>
+      <c r="H39" t="n">
+        <v>8.82</v>
+      </c>
+      <c r="I39" t="b">
+        <v>1</v>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
+      </c>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="n">
+        <v>342186</v>
+      </c>
+      <c r="N39" t="n">
+        <v>6.19</v>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Massachusetts</t>
+        </is>
+      </c>
+      <c r="B40" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C40" t="n">
+        <v>110602</v>
+      </c>
+      <c r="D40" t="n">
+        <v>8243</v>
+      </c>
+      <c r="E40" t="n">
+        <v>10414</v>
+      </c>
+      <c r="F40" t="n">
+        <v>675</v>
+      </c>
+      <c r="G40" t="n">
+        <v>9.42</v>
+      </c>
+      <c r="H40" t="n">
+        <v>8.19</v>
+      </c>
+      <c r="I40" t="b">
+        <v>1</v>
+      </c>
+      <c r="J40" t="b">
+        <v>0</v>
+      </c>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="n">
+        <v>510558</v>
+      </c>
+      <c r="N40" t="n">
+        <v>7.48</v>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Wisconsin -- Milwaukee</t>
+        </is>
+      </c>
+      <c r="B41" s="2" t="n">
+        <v>44020</v>
+      </c>
+      <c r="C41" t="n">
+        <v>12834</v>
+      </c>
+      <c r="D41" t="n">
+        <v>358</v>
+      </c>
+      <c r="E41" t="n">
+        <v>3731</v>
+      </c>
+      <c r="F41" t="n">
+        <v>145</v>
+      </c>
+      <c r="G41" t="n">
+        <v>31.32</v>
+      </c>
+      <c r="H41" t="n">
+        <v>40.5</v>
+      </c>
+      <c r="I41" t="b">
+        <v>0</v>
+      </c>
+      <c r="J41" t="b">
+        <v>0</v>
+      </c>
+      <c r="K41" t="n">
+        <v>11914</v>
+      </c>
+      <c r="L41" t="n">
+        <v>358</v>
+      </c>
+      <c r="M41" t="n">
+        <v>252321</v>
+      </c>
+      <c r="N41" t="n">
+        <v>26.44</v>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Missouri</t>
+        </is>
+      </c>
+      <c r="B42" s="2" t="n">
+        <v>44009</v>
+      </c>
+      <c r="C42" t="n">
+        <v>20261</v>
+      </c>
+      <c r="D42" t="n">
+        <v>996</v>
+      </c>
+      <c r="E42" t="n">
+        <v>5758</v>
+      </c>
+      <c r="F42" t="n">
+        <v>246</v>
+      </c>
+      <c r="G42" t="n">
+        <v>49.66</v>
+      </c>
+      <c r="H42" t="n">
+        <v>38.56</v>
+      </c>
+      <c r="I42" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" t="b">
+        <v>1</v>
+      </c>
+      <c r="K42" t="n">
+        <v>11594</v>
+      </c>
+      <c r="L42" t="n">
+        <v>638</v>
+      </c>
+      <c r="M42" t="n">
+        <v>704896</v>
+      </c>
+      <c r="N42" t="n">
+        <v>11.57</v>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>Success!</t>
         </is>
       </c>
     </row>

</xml_diff>